<commit_message>
#2115 error when importing empty row (#2384)
* #2115 error when importing empty row

* #2115 test update

* #2115 remove empty rows

* #2115 remove extra instructions

* #2115 code cleanup
</commit_message>
<xml_diff>
--- a/tests/OSPSuite.Presentation.Tests/Data/IntegrationSampleUnitFromColumn.xlsx
+++ b/tests/OSPSuite.Presentation.Tests/Data/IntegrationSampleUnitFromColumn.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GeorgiosDaskalakis\Documents\GitHub\OSPSuite.Core\tests\OSPSuite.Presentation.Tests\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BenjaminMarianoPerez\source\repos\OSPSuite.Core\tests\OSPSuite.Presentation.Tests\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F65A59A-94EE-452A-A39D-C50F01168746}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E4EE7C7-5908-4FAE-B234-4E0B619F04E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4905" yWindow="-13650" windowWidth="21600" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -108,9 +108,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -148,7 +148,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -254,7 +254,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -396,7 +396,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -404,10 +404,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -446,38 +446,38 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="2">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="2">
-        <v>2</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>3</v>
-      </c>
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
+      <c r="A5" s="2">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="2">
+        <v>3</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
@@ -539,6 +539,12 @@
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
     </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>